<commit_message>
Atualização automática de SAO_GABRIEL.xlsx
</commit_message>
<xml_diff>
--- a/SAO_GABRIEL.xlsx
+++ b/SAO_GABRIEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5E80F57-F286-414F-AA2B-E54B04B10062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E65E867-C116-434A-9D60-B6B1F9DDCDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1231,7 +1231,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{B5B29ED2-54B6-4EA1-B19B-910C7CDF9F8A}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{6FE5F29A-E1D3-45F9-B9C3-CD176EE90B4B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1261,10 +1261,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{804CC63F-88B3-452E-A8E0-C757B27CAB11}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E20DFE5F-AFC0-4FB4-8712-9908230EF0D4}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1302,7 +1302,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00C6F377-C05D-44EC-84C9-6596A0F38268}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{965B2F00-B2E1-4B3C-912A-FC4D7DD4FFE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1365,7 +1365,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{532BCAE3-69DD-44CD-8A03-5C2AD995C043}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{556A2FDE-89A6-4C25-BEAD-B02EE749EB1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1384,7 +1384,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A704D61-432C-A8E5-69AC-9B2A75F455B9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{708988D1-52A3-4041-AFC0-A8259FCF0D2B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1433,7 +1433,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE46A193-F4E2-C4C7-C371-E84182D6A4BF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5875B91B-0DAA-EEB3-0952-FADA189A9B37}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1452,7 +1452,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9B8F989-C691-2AC2-C27E-61F30276C189}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFF5EF43-9F52-E585-EDAE-A19A1BA37976}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1483,7 +1483,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{866CCE3F-2DFE-44F9-B9B0-39E29E91DD92}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64390B54-35F8-776C-9C2E-DF4260FF5840}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1514,7 +1514,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97B4600F-5DD9-781D-4493-18D51DE5A61D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2634DA60-DCEB-53FB-82E8-802F189C3F6E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1557,7 +1557,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B9D3014-2451-46DD-8A1C-C43FD112FEF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{117EE01A-103A-4709-BB45-2943246206EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1595,7 +1595,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F13A19BB-28DF-4DE6-9526-7460A4171918}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90649E02-9736-418F-A390-6456BFFDEBBF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1638,7 +1638,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A82EA8C-724C-4847-A325-8696C3BDB315}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{250E0A4B-4D79-461E-A020-E9918D9E581E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1951,7 +1951,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D832F9-2F49-4D5D-9379-03A656A6EFC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358E7E50-DC7B-4841-8C78-0CA7B24A27E8}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>